<commit_message>
Working method keywords execute
</commit_message>
<xml_diff>
--- a/bin/com/qtpselenium/xls/Check Items.xlsx
+++ b/bin/com/qtpselenium/xls/Check Items.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>Result2</t>
+  </si>
+  <si>
+    <t>Result3</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -856,7 +862,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
@@ -864,6 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1251,7 +1258,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
@@ -1268,6 +1275,7 @@
     <col min="7" max="7" customWidth="true" width="19.7142857142857" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="7.69921875" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="7.69921875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1298,6 +1306,9 @@
       <c r="I1" t="s" s="8">
         <v>63</v>
       </c>
+      <c r="J1" t="s" s="9">
+        <v>64</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
@@ -1321,6 +1332,9 @@
       <c r="I2" t="s">
         <v>62</v>
       </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
@@ -1344,6 +1358,9 @@
       <c r="I3" t="s">
         <v>62</v>
       </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
@@ -1367,6 +1384,9 @@
       <c r="I4" t="s">
         <v>62</v>
       </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
@@ -1390,6 +1410,9 @@
       <c r="I5" t="s">
         <v>62</v>
       </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
@@ -1413,6 +1436,9 @@
       <c r="I6" t="s">
         <v>62</v>
       </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
@@ -1436,6 +1462,9 @@
       <c r="I7" t="s">
         <v>62</v>
       </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
@@ -1459,6 +1488,9 @@
       <c r="I8" t="s">
         <v>62</v>
       </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
@@ -1482,6 +1514,9 @@
       <c r="I9" t="s">
         <v>62</v>
       </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
@@ -1505,6 +1540,9 @@
       <c r="I10" t="s">
         <v>62</v>
       </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
@@ -1528,6 +1566,9 @@
       <c r="I11" t="s">
         <v>62</v>
       </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
@@ -1551,6 +1592,9 @@
       <c r="I12" t="s">
         <v>62</v>
       </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
@@ -1574,6 +1618,9 @@
       <c r="I13" t="s">
         <v>62</v>
       </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
@@ -1597,6 +1644,9 @@
       <c r="I14" t="s">
         <v>62</v>
       </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
@@ -1620,6 +1670,9 @@
       <c r="I15" t="s">
         <v>62</v>
       </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
@@ -1643,6 +1696,9 @@
       <c r="I16" t="s">
         <v>62</v>
       </c>
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
@@ -1665,6 +1721,9 @@
       </c>
       <c r="I17" t="s">
         <v>62</v>
+      </c>
+      <c r="J17" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1801,9 @@
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1832,7 +1893,9 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>